<commit_message>
1) Done - 2) in progress - data_inout.py update
</commit_message>
<xml_diff>
--- a/Docs/AOP_ML_diagram.xlsx
+++ b/Docs/AOP_ML_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\AOP_ML\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDE9802-1FEA-41F7-8916-F81D30F309DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC9263A-B395-4D6B-BC0E-81A279CC2BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDAB8857-9B94-4A1A-BE25-65B4E9604164}"/>
+    <workbookView xWindow="28680" yWindow="-7980" windowWidth="18240" windowHeight="28440" xr2:uid="{BDAB8857-9B94-4A1A-BE25-65B4E9604164}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>meas_generation.py</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>top_menu.py</t>
+  </si>
+  <si>
+    <t>verify_report.py</t>
+  </si>
+  <si>
+    <t>verify_query.py</t>
+  </si>
+  <si>
+    <t>i) self.list_probe 변경 시,</t>
+  </si>
+  <si>
+    <t>o) execute_query 실행</t>
+  </si>
+  <si>
+    <t>i) table내 str_sel_param &amp; probeId 선택 verify_report 버튼</t>
+  </si>
+  <si>
+    <t>o) _get_sequence 실행하여 table 업데이트</t>
   </si>
 </sst>
 </file>
@@ -242,50 +260,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,23 +432,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>201707</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>78440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>152995</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104381</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336177</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>25351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3">
+        <xdr:cNvPr id="5" name="그림 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADA617C6-A917-4793-1CC9-05F0B01A006C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8FE2E9C-A56E-D441-3B04-4A6F9D6B60F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -446,8 +464,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15822706" y="2812677"/>
-          <a:ext cx="4198318" cy="3163586"/>
+          <a:off x="11351560" y="5591734"/>
+          <a:ext cx="7552764" cy="5673117"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -756,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71AC3DA5-E89A-4A0A-8BD1-B9562B650DD9}">
-  <dimension ref="B1:N43"/>
+  <dimension ref="B1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -770,9 +788,10 @@
     <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="1" customWidth="1"/>
@@ -782,14 +801,14 @@
   <sheetData>
     <row r="1" spans="8:14" ht="15.75" thickBot="1"/>
     <row r="2" spans="8:14">
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="8:14" ht="15.75" thickBot="1">
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="8:14">
       <c r="J4" s="2"/>
@@ -800,40 +819,40 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="8:14">
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="13"/>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="8:14" ht="15.75" thickBot="1">
-      <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="8:14" ht="5.25" customHeight="1" thickBot="1">
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="8:14">
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="8:14" ht="15.75" thickBot="1">
-      <c r="H10" s="17"/>
-      <c r="J10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="J10" s="8"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="19"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="8:14">
       <c r="H11" s="5" t="s">
@@ -869,125 +888,149 @@
     </row>
     <row r="15" spans="8:14" ht="15.75" thickBot="1"/>
     <row r="16" spans="8:14">
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="5:12" ht="15.75" thickBot="1">
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="23" spans="5:12">
-      <c r="L23" s="20"/>
-    </row>
-    <row r="24" spans="5:12">
-      <c r="L24" s="20"/>
-    </row>
-    <row r="25" spans="5:12">
-      <c r="L25" s="20"/>
-    </row>
-    <row r="26" spans="5:12">
-      <c r="L26" s="20"/>
-    </row>
-    <row r="27" spans="5:12">
-      <c r="L27" s="20"/>
-    </row>
-    <row r="28" spans="5:12">
-      <c r="L28" s="20"/>
-    </row>
-    <row r="29" spans="5:12">
-      <c r="L29" s="20"/>
-    </row>
-    <row r="30" spans="5:12" ht="15.75" thickBot="1">
-      <c r="L30" s="20"/>
-    </row>
-    <row r="31" spans="5:12">
-      <c r="E31" s="6" t="s">
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" thickBot="1">
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.75" thickBot="1">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="E22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="L31" s="20"/>
-    </row>
-    <row r="32" spans="5:12" ht="15.75" thickBot="1">
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="L32" s="20"/>
+      <c r="F22" s="10"/>
+      <c r="I22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1">
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="I24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="I25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="I26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1">
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" s="6"/>
     </row>
     <row r="33" spans="2:12">
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="L33" s="20"/>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="6"/>
     </row>
     <row r="34" spans="2:12">
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="L34" s="20"/>
-    </row>
-    <row r="35" spans="2:12" ht="15.75" thickBot="1">
-      <c r="L35" s="20"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="L35" s="6"/>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L36" s="20"/>
-    </row>
-    <row r="37" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="L37" s="20"/>
-    </row>
-    <row r="38" spans="2:12">
-      <c r="B38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L38" s="20"/>
-    </row>
-    <row r="39" spans="2:12">
-      <c r="B39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L39" s="20"/>
-    </row>
-    <row r="40" spans="2:12">
-      <c r="L40" s="20"/>
-    </row>
-    <row r="41" spans="2:12">
-      <c r="L41" s="20"/>
-    </row>
-    <row r="42" spans="2:12">
-      <c r="L42" s="20"/>
-    </row>
-    <row r="43" spans="2:12">
-      <c r="L43" s="20"/>
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="L37" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="E31:F32"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="J16:K17"/>
+  <mergeCells count="13">
     <mergeCell ref="J6:K7"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="L9:L10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="J16:K17"/>
+    <mergeCell ref="I22:J23"/>
+    <mergeCell ref="I30:I31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>